<commit_message>
Update Libretto Nuovo Oridnamento.xlsx
</commit_message>
<xml_diff>
--- a/Libretto Nuovo Oridnamento.xlsx
+++ b/Libretto Nuovo Oridnamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bickpenna/GitHub/LibrettoEsami/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2EB7E0-B2F8-4E49-9FD8-BBEFB9E34843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD525255-7D04-9446-8C4F-2FD799C8F3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{60CC99F7-4A85-AF4D-AE18-150057B74713}"/>
   </bookViews>
@@ -468,6 +468,40 @@
     <xf numFmtId="14" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,46 +523,110 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4ABFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4ABFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4ABFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4ABFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -904,8 +1002,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:XFD1048551"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,26 +1040,26 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="H3" s="25" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -976,8 +1074,8 @@
         <v>1</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1036,8 +1134,8 @@
         <v>1</v>
       </c>
       <c r="F7" s="14"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1056,7 +1154,7 @@
       <c r="H8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="34" t="e">
+      <c r="I8" s="17" t="e">
         <f>INDEX(A:A,MATCH(MAX(F:F),F:F,0))</f>
         <v>#N/A</v>
       </c>
@@ -1079,7 +1177,7 @@
       <c r="H9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="18">
         <f>MAX(F4:F11,F14:F22,F25:F29)</f>
         <v>0</v>
       </c>
@@ -1099,15 +1197,15 @@
         <v>2</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="6"/>
       <c r="H11" s="1" t="s">
         <v>25</v>
@@ -1118,14 +1216,14 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
       <c r="H12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1166,8 +1264,8 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="14"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1238,8 +1336,8 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="14"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -1277,8 +1375,8 @@
         <v/>
       </c>
       <c r="F20" s="14"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -1306,11 +1404,11 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="6"/>
       <c r="H22" s="1" t="s">
         <v>48</v>
@@ -1321,14 +1419,14 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
       <c r="H23" s="1" t="s">
         <v>47</v>
       </c>
@@ -1350,8 +1448,8 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="10"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1387,8 +1485,8 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="14"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -1449,14 +1547,14 @@
       <c r="B30" s="1">
         <v>13</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="10"/>
-      <c r="H30" s="25" t="s">
+      <c r="H30" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I30" s="26"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -1465,7 +1563,7 @@
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="10"/>
@@ -1477,37 +1575,37 @@
       <c r="B32" s="1">
         <v>4</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="6"/>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="20"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1787,12 +1885,9 @@
     <sortCondition ref="E36:E47"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A34:E34"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="H24:I24"/>
@@ -1804,44 +1899,47 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A21">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Esami a Scelta Libera">
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Esami a Scelta Libera">
       <formula>NOT(ISERROR(SEARCH("Esami a Scelta Libera",A21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Esami a Scelta Libera">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Esami a Scelta Libera">
       <formula>NOT(ISERROR(SEARCH("Esami a Scelta Libera",A29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="4" priority="15">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>$C35&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:F10">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>$C4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:F21">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$C13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24:F29">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$C24&lt;&gt;""</formula>
+  <conditionalFormatting sqref="A36:F47">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>AND($C$21&lt;&gt;"",$C$29&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36:F47">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($C$21&lt;&gt;"",$C$29&lt;&gt;"")</formula>
+  <conditionalFormatting sqref="A24:F32">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$C24&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">

</xml_diff>